<commit_message>
Fixed xlrd newer version
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E7C937-55BC-4343-80FC-35A00E9FC1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Attorney</t>
   </si>
@@ -82,14 +91,26 @@
   </si>
   <si>
     <t>Donald J. Trump</t>
+  </si>
+  <si>
+    <t>Padi &amp; Sons</t>
+  </si>
+  <si>
+    <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>Acquire Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -131,7 +152,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,18 +432,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -550,9 +571,35 @@
         <v>43952</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>5555</v>
+      </c>
+      <c r="E5">
+        <v>2222</v>
+      </c>
+      <c r="G5">
+        <v>2222</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2">
+        <v>43953</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://www.ranker.com/review/baker-and-mckenzie/534060?ref=node_name&amp;pos=1&amp;a=0&amp;ltype=n&amp;l=407667&amp;g=1"/>
+    <hyperlink ref="A4" r:id="rId1" display="https://www.ranker.com/review/baker-and-mckenzie/534060?ref=node_name&amp;pos=1&amp;a=0&amp;ltype=n&amp;l=407667&amp;g=1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>